<commit_message>
Here is Dictionary for dataset
</commit_message>
<xml_diff>
--- a/docs/Dictionary for Program Budget Operating Budget Vs Expense.xlsx
+++ b/docs/Dictionary for Program Budget Operating Budget Vs Expense.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lflapple/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lflapple/Desktop/9440/cis9440hw12/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{739840A9-118B-E344-A6C1-55FE863ED6EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{449ADEEC-73FC-164F-A42D-01F12A933C83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14820" xr2:uid="{0BE51EDB-367A-0745-A9B8-C30E7E4145ED}"/>
   </bookViews>
@@ -198,7 +198,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -237,14 +237,6 @@
       <family val="2"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color rgb="FF0D0D0D"/>
       <name val="Arial"/>
@@ -274,25 +266,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -628,7 +617,7 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -638,17 +627,17 @@
     <col min="3" max="3" width="29.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="5" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>5</v>
       </c>
     </row>
@@ -656,20 +645,20 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="7"/>
+      <c r="B2" s="6"/>
       <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="8"/>
+      <c r="F2" s="7"/>
     </row>
     <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -678,28 +667,28 @@
       <c r="D3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="8"/>
+      <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -708,13 +697,13 @@
       <c r="D5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -723,13 +712,13 @@
       <c r="D6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -738,13 +727,13 @@
       <c r="D7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -753,13 +742,13 @@
       <c r="D8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -768,13 +757,13 @@
       <c r="D9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -783,13 +772,13 @@
       <c r="D10" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="6" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -798,13 +787,13 @@
       <c r="D11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="7"/>
     </row>
     <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -813,13 +802,13 @@
       <c r="D12" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="7"/>
     </row>
     <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="B13" s="6" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -828,39 +817,39 @@
       <c r="D13" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="7"/>
     </row>
     <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B14" s="7"/>
+      <c r="B14" s="6"/>
       <c r="C14" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="7"/>
     </row>
     <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B15" s="7"/>
+      <c r="B15" s="6"/>
       <c r="C15" s="2" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="7"/>
     </row>
     <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>40</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -869,13 +858,13 @@
       <c r="D16" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -884,39 +873,39 @@
       <c r="D17" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F17" s="8"/>
+      <c r="F17" s="7"/>
     </row>
     <row r="18" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="7"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="8"/>
+      <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B19" s="7"/>
+      <c r="B19" s="6"/>
       <c r="C19" s="2" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="F19" s="8"/>
+      <c r="F19" s="7"/>
     </row>
     <row r="20" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>50</v>
       </c>
       <c r="C20" s="2"/>

</xml_diff>